<commit_message>
Resolving conflict issues - Replaced files
</commit_message>
<xml_diff>
--- a/KatalonData/IWPTestData/VRelay25PaymentsExtension.xlsx
+++ b/KatalonData/IWPTestData/VRelay25PaymentsExtension.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t476046\Documents\katalon\VPS-Katalon\KatalonData\IWPTestData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\IWPTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{C4BFA823-FF9D-47E7-8388-2160B1142FF2}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{7F143880-D589-4840-A6E8-EE7456AF6FD8}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="8" firstSheet="6" windowHeight="12576" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
+    <workbookView activeTab="4" firstSheet="3" windowHeight="11490" windowWidth="15330" xWindow="12795" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="2670"/>
   </bookViews>
   <sheets>
     <sheet name="CCDeferredPlanCorp" r:id="rId1" sheetId="4"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3552" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3452" uniqueCount="219">
   <si>
     <t>Result</t>
   </si>
@@ -442,54 +442,6 @@
     <t>Fri Oct 25 01:15:55 IST 2024</t>
   </si>
   <si>
-    <t>Fri Oct 25 01:34:51 IST 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 01:36:27 IST 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 01:38:50 IST 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 01:40:26 IST 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 01:42:14 IST 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 01:43:50 IST 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 01:46:12 IST 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 01:47:48 IST 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 01:50:09 IST 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 01:51:55 IST 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 01:54:11 IST 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 01:55:58 IST 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 01:57:42 IST 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 01:59:29 IST 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 02:01:46 IST 2024</t>
-  </si>
-  <si>
-    <t>Fri Oct 25 02:03:34 IST 2024</t>
-  </si>
-  <si>
     <t>Fri Oct 25 02:05:50 IST 2024</t>
   </si>
   <si>
@@ -541,259 +493,235 @@
     <t>15</t>
   </si>
   <si>
+    <t>Wed Oct 30 14:48:42 IST 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 30 14:50:17 IST 2024</t>
+  </si>
+  <si>
+    <t>Tue Dec 03 18:57:27 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Dec 03 18:58:37 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Dec 03 19:00:04 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Dec 03 19:01:10 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Dec 03 19:02:16 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Dec 03 19:03:21 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Dec 03 19:04:48 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Dec 03 19:05:52 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Dec 03 19:07:20 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Dec 03 19:08:27 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Dec 03 19:09:57 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Dec 03 19:11:04 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Dec 03 19:12:10 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Dec 03 19:13:17 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Dec 03 19:14:47 EST 2024</t>
+  </si>
+  <si>
+    <t>Tue Dec 03 19:15:54 EST 2024</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Wed Oct 30 14:43:31 IST 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 30 14:45:09 IST 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 30 14:48:42 IST 2024</t>
-  </si>
-  <si>
-    <t>Wed Oct 30 14:50:17 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Dec 03 14:09:20 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Dec 03 14:10:31 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Dec 03 18:57:27 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Dec 03 18:58:37 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Dec 03 19:00:04 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Dec 03 19:01:10 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Dec 03 19:02:16 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Dec 03 19:03:21 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Dec 03 19:04:48 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Dec 03 19:05:52 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Dec 03 19:07:20 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Dec 03 19:08:27 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Dec 03 19:09:57 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Dec 03 19:11:04 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Dec 03 19:12:10 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Dec 03 19:13:17 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Dec 03 19:14:47 EST 2024</t>
-  </si>
-  <si>
-    <t>Tue Dec 03 19:15:54 EST 2024</t>
-  </si>
-  <si>
-    <t>Wed Feb 05 21:39:29 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 05 21:42:59 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 05 21:46:25 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 05 21:49:50 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 05 21:53:17 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 05 21:56:40 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 05 22:00:03 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 05 22:03:26 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 05 22:06:51 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 05 22:10:14 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 05 22:13:37 IST 2025</t>
-  </si>
-  <si>
-    <t>Wed Feb 05 22:17:02 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:10:08 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:11:37 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:13:17 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:14:52 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:16:28 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:17:56 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:19:29 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:20:51 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:22:24 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:23:33 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:24:43 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:25:53 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:27:26 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:28:36 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:30:10 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:31:20 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:32:53 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:34:18 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:36:41 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:38:03 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:39:35 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:40:58 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:42:30 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:43:53 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:45:27 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:46:41 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:48:12 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:49:27 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:50:44 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:51:59 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:53:31 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:54:45 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:56:17 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:57:28 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 14:59:02 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 15:00:17 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 15:01:29 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 15:02:41 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 15:04:16 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 15:05:29 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 15:08:18 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 15:13:30 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 15:16:18 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 15:17:51 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 15:19:11 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 15:20:44 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 15:22:04 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 15:23:25 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 15:24:58 IST 2025</t>
-  </si>
-  <si>
-    <t>Thu Feb 06 15:26:18 IST 2025</t>
+    <t>Mon Jan 20 19:57:31 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jan 20 19:58:40 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jan 20 19:59:45 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jan 20 20:00:49 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jan 20 20:01:53 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jan 20 20:02:59 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jan 20 20:04:04 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jan 20 20:05:34 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jan 20 20:07:13 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jan 20 20:08:52 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jan 20 20:10:31 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jan 20 20:11:38 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jan 20 20:12:45 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jan 20 20:13:53 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jan 20 20:15:02 EST 2025</t>
+  </si>
+  <si>
+    <t>Mon Jan 20 20:16:11 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 22 14:16:23 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 22 14:17:41 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 22 14:18:55 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 22 14:20:06 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 22 14:21:32 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 22 14:22:44 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 22 14:24:11 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 22 14:25:23 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 22 14:34:24 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 22 14:35:27 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 22 14:36:31 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 22 14:37:35 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 22 14:39:02 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 22 14:40:08 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 22 14:41:36 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 22 14:42:41 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 22 14:44:09 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 22 14:45:25 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 22 14:46:41 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 22 14:47:56 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 22 14:49:23 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 22 14:50:39 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 22 14:52:08 EST 2025</t>
+  </si>
+  <si>
+    <t>Wed Jan 22 14:53:27 EST 2025</t>
+  </si>
+  <si>
+    <t>Fri Jan 24 14:12:36 EST 2025</t>
+  </si>
+  <si>
+    <t>Fri Jan 24 14:13:56 EST 2025</t>
+  </si>
+  <si>
+    <t>Fri Jan 24 14:15:10 EST 2025</t>
+  </si>
+  <si>
+    <t>Fri Jan 24 14:16:24 EST 2025</t>
+  </si>
+  <si>
+    <t>Fri Jan 24 14:17:38 EST 2025</t>
+  </si>
+  <si>
+    <t>Fri Jan 24 14:18:52 EST 2025</t>
+  </si>
+  <si>
+    <t>Fri Jan 24 14:22:16 EST 2025</t>
+  </si>
+  <si>
+    <t>Fri Jan 24 14:23:22 EST 2025</t>
+  </si>
+  <si>
+    <t>Fri Jan 24 14:24:28 EST 2025</t>
+  </si>
+  <si>
+    <t>Fri Jan 24 14:25:34 EST 2025</t>
+  </si>
+  <si>
+    <t>Fri Jan 24 14:26:40 EST 2025</t>
+  </si>
+  <si>
+    <t>Fri Jan 24 14:27:46 EST 2025</t>
+  </si>
+  <si>
+    <t>Fri Jan 24 14:28:53 EST 2025</t>
+  </si>
+  <si>
+    <t>Fri Jan 24 14:30:09 EST 2025</t>
+  </si>
+  <si>
+    <t>Fri Jan 24 14:31:25 EST 2025</t>
+  </si>
+  <si>
+    <t>Fri Jan 24 14:32:42 EST 2025</t>
+  </si>
+  <si>
+    <t>Fri Jan 24 14:34:00 EST 2025</t>
+  </si>
+  <si>
+    <t>Fri Jan 24 14:35:17 EST 2025</t>
   </si>
 </sst>
 </file>
@@ -1163,13 +1091,13 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="29" max="29" bestFit="true" customWidth="true" width="9.44140625" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1258,12 +1186,12 @@
       <c r="AD1" s="3"/>
       <c r="AE1" s="3"/>
     </row>
-    <row ht="72" r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>225</v>
+        <v>169</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>56</v>
@@ -1344,12 +1272,12 @@
       <c r="AC2" s="2"/>
       <c r="AE2" s="4"/>
     </row>
-    <row ht="72" r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>226</v>
+        <v>170</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>56</v>
@@ -1441,9 +1369,9 @@
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1529,12 +1457,12 @@
         <v>54</v>
       </c>
     </row>
-    <row ht="72" r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>56</v>
@@ -1615,12 +1543,12 @@
         <v>27</v>
       </c>
     </row>
-    <row ht="72" r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>56</v>
@@ -1714,9 +1642,9 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1802,12 +1730,12 @@
         <v>54</v>
       </c>
     </row>
-    <row ht="72" r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>195</v>
+        <v>201</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>56</v>
@@ -1888,12 +1816,12 @@
         <v>27</v>
       </c>
     </row>
-    <row ht="72" r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>196</v>
+        <v>202</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>56</v>
@@ -1987,9 +1915,9 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2080,12 +2008,12 @@
       <c r="AD1" s="3"/>
       <c r="AE1" s="3"/>
     </row>
-    <row ht="72" r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>211</v>
+        <v>213</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>56</v>
@@ -2168,12 +2096,12 @@
       <c r="AC2" s="2"/>
       <c r="AE2" s="4"/>
     </row>
-    <row ht="72" r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>212</v>
+        <v>214</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>56</v>
@@ -2268,9 +2196,9 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2365,12 +2293,12 @@
         <v>54</v>
       </c>
     </row>
-    <row ht="72" r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>56</v>
@@ -2460,12 +2388,12 @@
         <v>27</v>
       </c>
     </row>
-    <row ht="72" r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>56</v>
@@ -2568,12 +2496,12 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" customWidth="true" width="29.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2673,12 +2601,12 @@
       <c r="AG1" s="3"/>
       <c r="AH1" s="3"/>
     </row>
-    <row ht="72" r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>56</v>
@@ -2770,12 +2698,12 @@
       <c r="AF2" s="2"/>
       <c r="AH2" s="4"/>
     </row>
-    <row ht="72" r="3" spans="1:34" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>216</v>
+        <v>218</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>56</v>
@@ -2879,9 +2807,9 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2976,12 +2904,12 @@
         <v>54</v>
       </c>
     </row>
-    <row ht="72" r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>199</v>
+        <v>205</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>56</v>
@@ -3071,12 +2999,12 @@
         <v>27</v>
       </c>
     </row>
-    <row ht="72" r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>200</v>
+        <v>206</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>56</v>
@@ -3179,12 +3107,12 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="23.21875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="23.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3273,12 +3201,12 @@
       <c r="AD1" s="1"/>
       <c r="AE1" s="1"/>
     </row>
-    <row ht="72" r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -3362,12 +3290,12 @@
       <c r="AD2" s="1"/>
       <c r="AE2" s="1"/>
     </row>
-    <row ht="72" r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -3461,9 +3389,9 @@
       <selection sqref="A1:AC3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3553,12 +3481,12 @@
       </c>
       <c r="AD1" s="1"/>
     </row>
-    <row ht="72" r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -3641,12 +3569,12 @@
       <c r="AC2" s="2"/>
       <c r="AD2" s="1"/>
     </row>
-    <row ht="72" r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -3741,9 +3669,9 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3829,12 +3757,12 @@
         <v>54</v>
       </c>
     </row>
-    <row ht="72" r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -3915,12 +3843,12 @@
         <v>27</v>
       </c>
     </row>
-    <row ht="72" r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -4014,9 +3942,9 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4111,12 +4039,12 @@
         <v>54</v>
       </c>
     </row>
-    <row ht="72" r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>56</v>
@@ -4206,12 +4134,12 @@
         <v>27</v>
       </c>
     </row>
-    <row ht="72" r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>56</v>
@@ -4314,20 +4242,20 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" style="2" width="8.77734375" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="8.77734375" collapsed="true"/>
-    <col min="8" max="22" style="2" width="8.77734375" collapsed="true"/>
-    <col min="23" max="23" bestFit="true" customWidth="true" style="2" width="9.77734375" collapsed="true"/>
-    <col min="24" max="25" bestFit="true" customWidth="true" style="2" width="8.77734375" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" style="2" width="9.77734375" collapsed="true"/>
-    <col min="27" max="31" style="2" width="8.77734375" collapsed="true"/>
-    <col min="32" max="32" bestFit="true" customWidth="true" style="2" width="8.77734375" collapsed="true"/>
-    <col min="33" max="16384" style="2" width="8.77734375" collapsed="true"/>
+    <col min="1" max="6" style="2" width="8.7109375" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="8.7109375" collapsed="true"/>
+    <col min="8" max="22" style="2" width="8.7109375" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="2" width="9.7109375" collapsed="true"/>
+    <col min="24" max="25" bestFit="true" customWidth="true" style="2" width="8.7109375" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="2" width="9.7109375" collapsed="true"/>
+    <col min="27" max="31" style="2" width="8.7109375" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" style="2" width="8.7109375" collapsed="true"/>
+    <col min="33" max="16384" style="2" width="8.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4425,12 +4353,12 @@
       <c r="AG1" s="3"/>
       <c r="AH1" s="3"/>
     </row>
-    <row ht="72" r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>229</v>
+        <v>173</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>56</v>
@@ -4520,12 +4448,12 @@
       <c r="AG2"/>
       <c r="AH2" s="4"/>
     </row>
-    <row ht="72" r="3" spans="1:34" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>230</v>
+        <v>174</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>56</v>
@@ -4626,12 +4554,12 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="17.21875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="17.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4731,12 +4659,12 @@
       <c r="AG1" s="3"/>
       <c r="AH1" s="3"/>
     </row>
-    <row ht="72" r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>56</v>
@@ -4828,12 +4756,12 @@
       <c r="AF2" s="2"/>
       <c r="AH2" s="4"/>
     </row>
-    <row ht="72" r="3" spans="1:34" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>56</v>
@@ -4937,9 +4865,9 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5034,12 +4962,12 @@
         <v>54</v>
       </c>
     </row>
-    <row ht="72" r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>197</v>
+        <v>203</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>56</v>
@@ -5129,12 +5057,12 @@
         <v>27</v>
       </c>
     </row>
-    <row ht="72" r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>198</v>
+        <v>204</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>56</v>
@@ -5237,9 +5165,9 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5337,12 +5265,12 @@
         <v>65</v>
       </c>
     </row>
-    <row ht="72" r="2" spans="1:32" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>241</v>
+        <v>137</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>56</v>
@@ -5431,12 +5359,12 @@
       </c>
       <c r="AF2" s="2"/>
     </row>
-    <row ht="72" r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>242</v>
+        <v>138</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>56</v>
@@ -5538,9 +5466,9 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5626,12 +5554,12 @@
         <v>54</v>
       </c>
     </row>
-    <row ht="72" r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>238</v>
+        <v>134</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -5710,12 +5638,12 @@
         <v>27</v>
       </c>
     </row>
-    <row ht="72" r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>239</v>
+        <v>135</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -5807,9 +5735,9 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -5907,7 +5835,7 @@
         <v>65</v>
       </c>
     </row>
-    <row ht="72" r="2" spans="1:32" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -6001,12 +5929,12 @@
       </c>
       <c r="AF2" s="2"/>
     </row>
-    <row ht="72" r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>240</v>
+        <v>136</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>56</v>
@@ -6108,9 +6036,9 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6199,12 +6127,12 @@
         <v>65</v>
       </c>
     </row>
-    <row ht="72" r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>236</v>
+        <v>132</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>56</v>
@@ -6284,12 +6212,12 @@
       </c>
       <c r="AC2" s="2"/>
     </row>
-    <row ht="72" r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>237</v>
+        <v>133</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>56</v>
@@ -6382,9 +6310,9 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6473,12 +6401,12 @@
         <v>65</v>
       </c>
     </row>
-    <row ht="72" r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>141</v>
+        <v>125</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>56</v>
@@ -6554,12 +6482,12 @@
       </c>
       <c r="AC2" s="2"/>
     </row>
-    <row ht="72" r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>233</v>
+        <v>126</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>56</v>
@@ -6648,9 +6576,9 @@
       <selection activeCell="A3" sqref="A3:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -6736,12 +6664,12 @@
         <v>54</v>
       </c>
     </row>
-    <row ht="72" r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>143</v>
+        <v>127</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -6816,7 +6744,7 @@
         <v>27</v>
       </c>
     </row>
-    <row ht="72" r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -6909,9 +6837,9 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7006,12 +6934,12 @@
         <v>54</v>
       </c>
     </row>
-    <row ht="72" r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>128</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>56</v>
@@ -7095,12 +7023,12 @@
         <v>27</v>
       </c>
     </row>
-    <row ht="72" r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>234</v>
+        <v>129</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>56</v>
@@ -7197,9 +7125,9 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7294,12 +7222,12 @@
         <v>54</v>
       </c>
     </row>
-    <row ht="72" r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>56</v>
@@ -7383,12 +7311,12 @@
         <v>27</v>
       </c>
     </row>
-    <row ht="72" r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>235</v>
+        <v>131</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>56</v>
@@ -7485,9 +7413,9 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:34" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7585,12 +7513,12 @@
       <c r="AG1" s="3"/>
       <c r="AH1" s="3"/>
     </row>
-    <row ht="72" r="2" spans="1:34" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>231</v>
+        <v>175</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>56</v>
@@ -7680,12 +7608,12 @@
       <c r="AF2" s="2"/>
       <c r="AH2" s="4"/>
     </row>
-    <row ht="72" r="3" spans="1:34" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:34" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>232</v>
+        <v>176</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>56</v>
@@ -7786,9 +7714,9 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -7874,7 +7802,7 @@
         <v>54</v>
       </c>
     </row>
-    <row ht="72" r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -7956,7 +7884,7 @@
         <v>27</v>
       </c>
     </row>
-    <row ht="72" r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -8051,9 +7979,9 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8139,7 +8067,7 @@
         <v>54</v>
       </c>
     </row>
-    <row ht="72" r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -8221,7 +8149,7 @@
         <v>27</v>
       </c>
     </row>
-    <row ht="72" r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -8316,9 +8244,9 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8413,7 +8341,7 @@
         <v>54</v>
       </c>
     </row>
-    <row ht="72" r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -8504,7 +8432,7 @@
         <v>27</v>
       </c>
     </row>
-    <row ht="72" r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -8608,9 +8536,9 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8696,7 +8624,7 @@
         <v>54</v>
       </c>
     </row>
-    <row ht="72" r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -8778,7 +8706,7 @@
         <v>27</v>
       </c>
     </row>
-    <row ht="72" r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -8873,9 +8801,9 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -8961,7 +8889,7 @@
         <v>54</v>
       </c>
     </row>
-    <row ht="72" r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>70</v>
       </c>
@@ -9043,7 +8971,7 @@
         <v>27</v>
       </c>
     </row>
-    <row ht="72" r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>70</v>
       </c>
@@ -9138,9 +9066,9 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9235,7 +9163,7 @@
         <v>54</v>
       </c>
     </row>
-    <row ht="72" r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -9326,7 +9254,7 @@
         <v>27</v>
       </c>
     </row>
-    <row ht="72" r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -9430,9 +9358,9 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9527,7 +9455,7 @@
         <v>54</v>
       </c>
     </row>
-    <row ht="72" r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -9618,7 +9546,7 @@
         <v>27</v>
       </c>
     </row>
-    <row ht="72" r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -9722,9 +9650,9 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9810,7 +9738,7 @@
         <v>54</v>
       </c>
     </row>
-    <row ht="72" r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -9892,7 +9820,7 @@
         <v>27</v>
       </c>
     </row>
-    <row ht="72" r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -9987,9 +9915,9 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10075,7 +10003,7 @@
         <v>54</v>
       </c>
     </row>
-    <row ht="72" r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -10157,7 +10085,7 @@
         <v>27</v>
       </c>
     </row>
-    <row ht="72" r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -10252,9 +10180,9 @@
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10349,7 +10277,7 @@
         <v>54</v>
       </c>
     </row>
-    <row ht="72" r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -10440,7 +10368,7 @@
         <v>27</v>
       </c>
     </row>
-    <row ht="72" r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -10544,12 +10472,12 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" style="2" width="8.77734375" collapsed="true"/>
+    <col min="1" max="16384" style="2" width="8.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:30" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10637,12 +10565,12 @@
       <c r="AC1" s="3"/>
       <c r="AD1" s="1"/>
     </row>
-    <row ht="72" r="2" spans="1:30" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>227</v>
+        <v>171</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -10722,12 +10650,12 @@
       </c>
       <c r="AD2" s="1"/>
     </row>
-    <row ht="72" r="3" spans="1:30" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>228</v>
+        <v>172</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -10822,9 +10750,9 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10919,7 +10847,7 @@
         <v>54</v>
       </c>
     </row>
-    <row ht="72" r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -11010,7 +10938,7 @@
         <v>27</v>
       </c>
     </row>
-    <row ht="72" r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -11114,9 +11042,9 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11211,7 +11139,7 @@
         <v>54</v>
       </c>
     </row>
-    <row ht="72" r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
@@ -11302,7 +11230,7 @@
         <v>27</v>
       </c>
     </row>
-    <row ht="72" r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -11402,22 +11330,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA69CD0F-BD47-4004-A91B-17A22C7F7735}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="6" style="2" width="8.88671875" collapsed="true"/>
+    <col min="1" max="6" style="2" width="8.85546875" collapsed="true"/>
     <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="9.0" collapsed="true"/>
-    <col min="8" max="19" style="2" width="8.88671875" collapsed="true"/>
+    <col min="8" max="19" style="2" width="8.85546875" collapsed="true"/>
     <col min="20" max="20" bestFit="true" customWidth="true" style="2" width="10.0" collapsed="true"/>
     <col min="21" max="22" bestFit="true" customWidth="true" style="2" width="9.0" collapsed="true"/>
     <col min="23" max="23" bestFit="true" customWidth="true" style="2" width="10.0" collapsed="true"/>
-    <col min="24" max="16384" style="2" width="8.88671875" collapsed="true"/>
+    <col min="24" max="16384" style="2" width="8.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11503,12 +11431,12 @@
         <v>54</v>
       </c>
     </row>
-    <row ht="72" r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>217</v>
+        <v>161</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>56</v>
@@ -11583,12 +11511,12 @@
         <v>27</v>
       </c>
     </row>
-    <row ht="72" r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>218</v>
+        <v>162</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>56</v>
@@ -11676,9 +11604,9 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11764,12 +11692,12 @@
         <v>54</v>
       </c>
     </row>
-    <row ht="72" r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>219</v>
+        <v>163</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -11844,12 +11772,12 @@
         <v>27</v>
       </c>
     </row>
-    <row ht="72" r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>220</v>
+        <v>164</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -11937,9 +11865,9 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12034,12 +11962,12 @@
         <v>54</v>
       </c>
     </row>
-    <row ht="72" r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>221</v>
+        <v>165</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>56</v>
@@ -12123,12 +12051,12 @@
         <v>27</v>
       </c>
     </row>
-    <row ht="72" r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>222</v>
+        <v>166</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>56</v>
@@ -12225,9 +12153,9 @@
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12322,12 +12250,12 @@
         <v>54</v>
       </c>
     </row>
-    <row ht="72" r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>223</v>
+        <v>167</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>56</v>
@@ -12411,12 +12339,12 @@
         <v>27</v>
       </c>
     </row>
-    <row ht="72" r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>224</v>
+        <v>168</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>56</v>
@@ -12509,13 +12437,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E59C18C8-BC16-4EF9-ABC9-D44DBC5FD391}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row ht="28.8" r="1" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="30" r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -12601,21 +12529,21 @@
         <v>54</v>
       </c>
     </row>
-    <row ht="72" r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="75" r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>70</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>142</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>156</v>
+        <v>140</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>29</v>
@@ -12657,21 +12585,21 @@
       <c r="AA2" s="1"/>
       <c r="AB2" s="1"/>
     </row>
-    <row ht="72" r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row ht="75" r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>70</v>
       </c>
       <c r="B3" t="s">
-        <v>162</v>
+        <v>143</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>155</v>
+        <v>139</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>157</v>
+        <v>141</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>72</v>

</xml_diff>

<commit_message>
Updated BWP SelIDE Test Cases and created BWP-Non-BootStrap-SelIDE Test Suite
</commit_message>
<xml_diff>
--- a/KatalonData/IWPTestData/VRelay25PaymentsExtension.xlsx
+++ b/KatalonData/IWPTestData/VRelay25PaymentsExtension.xlsx
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4446" uniqueCount="440">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4542" uniqueCount="464">
   <si>
     <t>Result</t>
   </si>
@@ -1388,6 +1388,78 @@
   </si>
   <si>
     <t>Fri Apr 25 09:19:59 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 05 14:25:34 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 05 14:26:00 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 05 15:18:59 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 05 15:19:26 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 05 15:21:42 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 05 15:22:09 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 05 15:23:18 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 05 15:23:43 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 05 15:24:50 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 05 15:25:15 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 05 15:27:14 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 05 15:27:40 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 05 15:46:31 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 05 15:46:57 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 05 15:55:13 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 05 15:55:39 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 05 16:03:32 EDT 2025</t>
+  </si>
+  <si>
+    <t>Tue Aug 05 16:03:58 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 07 15:06:18 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 07 15:06:46 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 07 15:07:32 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 07 15:07:58 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 07 15:09:04 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 07 15:09:29 EDT 2025</t>
   </si>
 </sst>
 </file>
@@ -5375,7 +5447,7 @@
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>358</v>
+        <v>440</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -5461,7 +5533,7 @@
         <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>359</v>
+        <v>441</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -6268,7 +6340,7 @@
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>362</v>
+        <v>458</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>56</v>
@@ -6363,7 +6435,7 @@
         <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>363</v>
+        <v>459</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>56</v>
@@ -12998,7 +13070,7 @@
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>384</v>
+        <v>462</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -13078,7 +13150,7 @@
         <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>385</v>
+        <v>463</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>

</xml_diff>

<commit_message>
Display CF changes Added delays
</commit_message>
<xml_diff>
--- a/KatalonData/IWPTestData/VRelay25PaymentsExtension.xlsx
+++ b/KatalonData/IWPTestData/VRelay25PaymentsExtension.xlsx
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4646" uniqueCount="481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4662" uniqueCount="485">
   <si>
     <t>Result</t>
   </si>
@@ -1511,6 +1511,18 @@
   </si>
   <si>
     <t>Fri Aug 22 03:52:12 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 02 19:28:40 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 02 19:30:22 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 02 19:44:19 IST 2025</t>
+  </si>
+  <si>
+    <t>Tue Sep 02 19:45:59 IST 2025</t>
   </si>
 </sst>
 </file>
@@ -12977,10 +12989,10 @@
     </row>
     <row ht="72" r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>428</v>
+        <v>481</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>56</v>
@@ -13060,7 +13072,7 @@
         <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>429</v>
+        <v>482</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>56</v>
@@ -13241,7 +13253,7 @@
         <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>430</v>
+        <v>483</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -13321,7 +13333,7 @@
         <v>55</v>
       </c>
       <c r="B3" t="s">
-        <v>431</v>
+        <v>484</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>

</xml_diff>